<commit_message>
Refactor and adjustments in parametrization
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54364f94d6d94729/Knowledge/UERJ/Aulas/Dissertação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="413" documentId="8_{D7F9342F-DC74-4DD3-8296-41704BD9204A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2F0B7EC-1078-4F70-BD78-F8708EC80D16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48B36D3-09BB-4350-BFE7-FA2E0EF27E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
@@ -327,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -374,6 +374,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,16 +401,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +417,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -708,48 +703,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="25" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -759,8 +754,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -794,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="5">
-        <v>0.47399999999999998</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="10"/>
@@ -819,7 +814,7 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="5">
-        <v>0.754</v>
+        <v>0.747</v>
       </c>
       <c r="J5" s="10"/>
     </row>
@@ -1000,48 +995,48 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="22" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="25" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1051,8 +1046,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1096,7 +1091,7 @@
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="3">
         <v>0.50600000000000001</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1109,7 +1104,7 @@
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="4" t="s">
         <v>8</v>
       </c>
@@ -1141,6 +1136,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A13:E13"/>
@@ -1153,18 +1160,6 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1175,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1191,48 +1186,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="25" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1242,8 +1237,8 @@
       <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1277,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="7">
-        <v>0.55069999999999997</v>
+        <v>0.54869999999999997</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="13"/>
@@ -1483,48 +1478,48 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="22" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="25" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1534,8 +1529,8 @@
       <c r="E15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1624,6 +1619,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1636,18 +1643,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes and refatoring on multitarget training
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48B36D3-09BB-4350-BFE7-FA2E0EF27E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49CF20A-3226-4A51-916E-16DC3D0175CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
     <sheet name="F1-Score" sheetId="1" r:id="rId2"/>
+    <sheet name="Files and experiments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
   <si>
     <t>DA Models</t>
   </si>
@@ -59,9 +60,6 @@
     <t>No Domain Adaptation</t>
   </si>
   <si>
-    <t>DANN</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -90,6 +88,84 @@
   </si>
   <si>
     <t>Multi target - TensorFlow 2</t>
+  </si>
+  <si>
+    <t>DANN + CVA - Evaluation on Source:</t>
+  </si>
+  <si>
+    <t>RO:</t>
+  </si>
+  <si>
+    <t>1-Tr: RO, Ts: RO (baseline)</t>
+  </si>
+  <si>
+    <t>2-Tr: RO-&gt;PA,MA, Ts: PA (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>3-Tr: RO-&gt;PA,MA, Ts: MA (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>4-Tr: RO-&gt;PA,MA, Ts: RO (domain adaptation multi-target validating on source)</t>
+  </si>
+  <si>
+    <t>MA:</t>
+  </si>
+  <si>
+    <t>1-Tr: MA, Ts: MA (baseline)</t>
+  </si>
+  <si>
+    <t>2-Tr: MA-&gt;RO,PA, Ts: RO (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>3-Tr: MA-&gt;RO,PA, Ts: PA (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>4-Tr: MA-&gt;RO,PA, Ts: MA (domain adaptation multi-target validating on source)</t>
+  </si>
+  <si>
+    <t>PA:</t>
+  </si>
+  <si>
+    <t>1-Tr: PA, Ts: PA (baseline)</t>
+  </si>
+  <si>
+    <t>2-Tr: PA-&gt;RO,MA, Ts: RO (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>3-Tr: PA-&gt;RO,MA, Ts: MA (domain adaptation multi-target)</t>
+  </si>
+  <si>
+    <t>4-Tr: PA-&gt;RO,MA, Ts: PA (domain adaptation multi-target validating on source)</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Checkpoints</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Amazon_RO_DeepLab_None_Amazon_RO</t>
+  </si>
+  <si>
+    <t>results_tr_Amazon_RO_DeepLab_None_Amazon_RO_multi_Amazon_RO</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Amazon_PA_DeepLab_None_Amazon_PA</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Cerrado_MA_DeepLab_None_Cerrado_MA</t>
+  </si>
+  <si>
+    <t>results_tr_Amazon_PA_DeepLab_None_Amazon_PA_multi_Amazon_PA</t>
+  </si>
+  <si>
+    <t>results_tr_Cerrado_MA_DeepLab_None_Cerrado_MA_multi_Cerrado_MA</t>
+  </si>
+  <si>
+    <t>DANN (Unbalanced)</t>
   </si>
 </sst>
 </file>
@@ -116,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +223,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -322,12 +404,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -355,7 +476,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,12 +488,67 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,24 +558,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -695,7 +854,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
@@ -703,48 +862,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="22" t="s">
+      <c r="A1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -754,8 +913,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -767,7 +926,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -782,20 +941,20 @@
       <c r="E4" s="10">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="33" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="5">
-        <v>0.47799999999999998</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -808,18 +967,18 @@
       <c r="E5" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="5">
-        <v>0.747</v>
+      <c r="I5" s="45">
+        <v>0.85899999999999999</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -832,25 +991,25 @@
       <c r="E6" s="11">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="11">
-        <v>0.77600000000000002</v>
+      <c r="J6" s="46">
+        <v>0.90600000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>7</v>
+      <c r="A7" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3">
         <v>0.56100000000000005</v>
@@ -858,20 +1017,20 @@
       <c r="E7" s="10">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>7</v>
+      <c r="F7" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -879,23 +1038,23 @@
         <v>0.317</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="10">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -906,27 +1065,27 @@
         <v>0.77200000000000002</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="33"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <v>0.61499999999999999</v>
@@ -934,20 +1093,20 @@
       <c r="E10" s="10">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>9</v>
+      <c r="F10" s="33" t="s">
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -955,23 +1114,23 @@
         <v>0.36399999999999999</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="10">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,61 +1141,61 @@
         <v>0.79400000000000004</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="33"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="28" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1046,8 +1205,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1059,107 +1218,165 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>9</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3">
         <v>0.50600000000000001</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="10">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="33"/>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.437</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="33"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15">
-        <v>0.437</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="H20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="A16:A18"/>
+  <mergeCells count="26">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A19:A21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F10:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1171,7 +1388,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F7" sqref="F7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1186,71 +1403,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="22" t="s">
+      <c r="A1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1265,20 +1482,20 @@
       <c r="E4" s="13">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="33" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="7">
-        <v>0.54869999999999997</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1291,18 +1508,18 @@
       <c r="E5" s="13">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="7">
-        <v>0.67849999999999999</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1312,28 +1529,28 @@
       <c r="D6" s="6">
         <v>0.6754</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="18">
-        <v>0.74060000000000004</v>
+      <c r="J6" s="17">
+        <v>0.82250000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>7</v>
+      <c r="A7" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="6">
         <v>0.4728</v>
@@ -1341,20 +1558,20 @@
       <c r="E7" s="13">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>7</v>
+      <c r="F7" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1362,23 +1579,23 @@
         <v>0.31850000000000001</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="13">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1389,27 +1606,27 @@
         <v>0.67820000000000003</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="33"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6">
         <v>0.53380000000000005</v>
@@ -1417,20 +1634,20 @@
       <c r="E10" s="13">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>9</v>
+      <c r="F10" s="33" t="s">
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1438,23 +1655,23 @@
         <v>0.376</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="13">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1465,172 +1682,160 @@
         <v>0.69810000000000005</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="33"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="28" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>9</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="6">
         <v>0.50270000000000004</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="13">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="19">
+        <v>10</v>
+      </c>
+      <c r="C18" s="18">
         <v>0.41060000000000002</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="18">
         <v>0.45789999999999997</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="21"/>
+      <c r="E18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="35"/>
       <c r="G18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="16" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1643,6 +1848,18 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1651,4 +1868,128 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46470600-F60B-4355-835B-9BD29A947D16}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjustments and bugfixes in training step, optimizer learning rate and charts creation
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49CF20A-3226-4A51-916E-16DC3D0175CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E97913-14AC-455C-90E4-AC7105665715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="44">
   <si>
     <t>DA Models</t>
   </si>
@@ -147,25 +147,28 @@
     <t>Checkpoints</t>
   </si>
   <si>
-    <t>checkpoint_tr_Amazon_RO_DeepLab_None_Amazon_RO</t>
-  </si>
-  <si>
-    <t>results_tr_Amazon_RO_DeepLab_None_Amazon_RO_multi_Amazon_RO</t>
-  </si>
-  <si>
-    <t>checkpoint_tr_Amazon_PA_DeepLab_None_Amazon_PA</t>
-  </si>
-  <si>
-    <t>checkpoint_tr_Cerrado_MA_DeepLab_None_Cerrado_MA</t>
-  </si>
-  <si>
-    <t>results_tr_Amazon_PA_DeepLab_None_Amazon_PA_multi_Amazon_PA</t>
-  </si>
-  <si>
-    <t>results_tr_Cerrado_MA_DeepLab_None_Cerrado_MA_multi_Cerrado_MA</t>
-  </si>
-  <si>
     <t>DANN (Unbalanced)</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Cerrado_MA_classification_Cerrado_MA</t>
+  </si>
+  <si>
+    <t>results_tr_Cerrado_MA_classification_Cerrado_MA</t>
+  </si>
+  <si>
+    <t>results_tr_Amazon_RO_classification_Amazon_RO</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Amazon_RO_classification_Amazon_RO</t>
+  </si>
+  <si>
+    <t>checkpoint_tr_Amazon_PA_classification_Amazon_PA</t>
+  </si>
+  <si>
+    <t>results_tr_Amazon_PA_classification_Amazon_PA</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +232,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -448,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,6 +537,38 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -531,35 +578,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,7 +862,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -853,57 +871,57 @@
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="42" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="39" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -913,8 +931,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -926,7 +944,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -941,20 +959,22 @@
       <c r="E4" s="10">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="45" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="I4" s="3"/>
+      <c r="H4" s="11">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.27</v>
+      </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -967,18 +987,18 @@
       <c r="E5" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="45">
-        <v>0.85899999999999999</v>
+      <c r="I5" s="11">
+        <v>0.89300000000000002</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -991,19 +1011,19 @@
       <c r="E6" s="11">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="46">
-        <v>0.90600000000000003</v>
+      <c r="J6" s="11">
+        <v>0.88400000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>42</v>
+      <c r="A7" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1017,8 +1037,8 @@
       <c r="E7" s="10">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>42</v>
+      <c r="F7" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -1030,7 +1050,7 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1043,7 +1063,7 @@
       <c r="E8" s="10">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1074,7 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1067,7 +1087,7 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1078,7 +1098,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1093,7 +1113,7 @@
       <c r="E10" s="10">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1106,7 +1126,7 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1119,7 +1139,7 @@
       <c r="E11" s="10">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1150,7 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1163,7 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1154,48 +1174,48 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="36" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="39" t="s">
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1205,8 +1225,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1238,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1233,7 +1253,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1246,7 +1266,7 @@
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1259,7 +1279,7 @@
       <c r="E17" s="10">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1270,7 +1290,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1303,7 @@
       <c r="E18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1294,12 +1314,12 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="24"/>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="46" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="24" t="s">
@@ -1314,12 +1334,12 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="33"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1332,12 +1352,12 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="14"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="35"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="14" t="s">
         <v>10</v>
       </c>
@@ -1351,24 +1371,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F19:F21"/>
@@ -1377,6 +1379,24 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1387,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1403,48 +1423,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="42" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="39" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1454,8 +1474,8 @@
       <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1487,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1482,20 +1502,24 @@
       <c r="E4" s="13">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="45" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="7">
-        <v>0.68500000000000005</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="13"/>
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.29549999999999998</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.4995</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1508,18 +1532,22 @@
       <c r="E5" s="13">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6">
+        <v>0.39489999999999997</v>
+      </c>
       <c r="I5" s="7">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="J5" s="13"/>
+        <v>0.81520000000000004</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.44090000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1532,19 +1560,23 @@
       <c r="E6" s="17">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="6">
+        <v>0.47660000000000002</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.70720000000000005</v>
+      </c>
       <c r="J6" s="17">
-        <v>0.82250000000000001</v>
+        <v>0.6976</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>42</v>
+      <c r="A7" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1558,8 +1590,8 @@
       <c r="E7" s="13">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>42</v>
+      <c r="F7" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -1571,7 +1603,7 @@
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1616,7 @@
       <c r="E8" s="13">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1595,7 +1627,7 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1608,7 +1640,7 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1651,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1634,7 +1666,7 @@
       <c r="E10" s="13">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1643,11 +1675,13 @@
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1660,7 +1694,7 @@
       <c r="E11" s="13">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1671,7 +1705,7 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1684,7 +1718,7 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1695,48 +1729,48 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="36" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="39" t="s">
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1746,8 +1780,8 @@
       <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1793,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1774,7 +1808,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1787,7 +1821,7 @@
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,7 +1834,7 @@
       <c r="E17" s="13">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1811,7 +1845,7 @@
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1824,7 +1858,7 @@
       <c r="E18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1836,6 +1870,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1848,18 +1894,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1874,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46470600-F60B-4355-835B-9BD29A947D16}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1906,10 +1940,10 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1936,11 +1970,11 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
+      <c r="B12" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1967,11 +2001,11 @@
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
+      <c r="B19" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1991,5 +2025,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scripts for computing metrics for all cross-domain combinations
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E97913-14AC-455C-90E4-AC7105665715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70550E9-802D-48E9-945F-127AF8C6D424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
   <si>
     <t>DA Models</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>results_tr_Amazon_PA_classification_Amazon_PA</t>
-  </si>
-  <si>
-    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1405,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1675,8 +1672,8 @@
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="35" t="s">
-        <v>43</v>
+      <c r="I10" s="35">
+        <v>0.40379999999999999</v>
       </c>
       <c r="J10" s="13"/>
     </row>
@@ -1698,11 +1695,15 @@
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>0.24479999999999999</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="13">
+        <v>0.33129999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="45"/>

</xml_diff>

<commit_message>
Improvements on charts and new scripts for multi-target training
- Improvements on charts generation;
- Main scripts to start multi target training;
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70550E9-802D-48E9-945F-127AF8C6D424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B19A734-44B5-4255-8A42-2517EB9D94C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="43">
   <si>
     <t>DA Models</t>
   </si>
@@ -192,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +241,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -460,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -536,8 +542,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,32 +578,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -858,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J5" activeCellId="1" sqref="J11 J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -877,48 +885,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="36" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -928,8 +936,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -941,7 +949,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -956,7 +964,7 @@
       <c r="E4" s="10">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="35" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -965,13 +973,15 @@
       <c r="H4" s="11">
         <v>0.71599999999999997</v>
       </c>
-      <c r="I4" s="3">
-        <v>0.27</v>
-      </c>
-      <c r="J4" s="10"/>
+      <c r="I4" s="47">
+        <v>0.35</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.67400000000000004</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -984,18 +994,22 @@
       <c r="E5" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="45"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="47">
+        <v>0.35499999999999998</v>
+      </c>
       <c r="I5" s="11">
         <v>0.89300000000000002</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="48">
+        <v>0.76100000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1008,18 +1022,22 @@
       <c r="E6" s="11">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="3">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="I6" s="47">
+        <v>0.81299999999999994</v>
+      </c>
       <c r="J6" s="11">
         <v>0.88400000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1034,7 +1052,7 @@
       <c r="E7" s="10">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="35" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1043,11 +1061,15 @@
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,18 +1082,22 @@
       <c r="E8" s="10">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="45"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1084,18 +1110,22 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="45"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1110,7 +1140,7 @@
       <c r="E10" s="10">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1119,11 +1149,15 @@
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="47">
+        <v>0.433</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.59799999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1136,18 +1170,22 @@
       <c r="E11" s="10">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="47">
+        <v>0.24199999999999999</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="48">
+        <v>0.74299999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1160,59 +1198,63 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="3">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="I12" s="47">
+        <v>0.81100000000000005</v>
+      </c>
       <c r="J12" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="39" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="42" t="s">
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1222,8 +1264,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1277,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1250,7 +1292,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1263,7 +1305,7 @@
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1276,7 +1318,7 @@
       <c r="E17" s="10">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="45"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1287,7 +1329,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="45"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1342,7 @@
       <c r="E18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="45"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1311,12 +1353,12 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="24"/>
       <c r="C19" s="28"/>
       <c r="D19" s="29"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="36" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="24" t="s">
@@ -1331,12 +1373,12 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="45"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="45"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1349,12 +1391,12 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="14"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="47"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="14" t="s">
         <v>10</v>
       </c>
@@ -1368,6 +1410,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F19:F21"/>
@@ -1376,24 +1436,6 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1404,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1420,48 +1462,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="36" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1471,8 +1513,8 @@
       <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1526,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1499,7 +1541,7 @@
       <c r="E4" s="13">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="35" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1516,7 +1558,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1529,7 +1571,7 @@
       <c r="E5" s="13">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="45"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1544,7 +1586,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1557,7 +1599,7 @@
       <c r="E6" s="17">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +1614,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1587,7 +1629,7 @@
       <c r="E7" s="13">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="35" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1596,11 +1638,15 @@
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="13"/>
+      <c r="I7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1613,18 +1659,22 @@
       <c r="E8" s="13">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="45"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1637,18 +1687,22 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="45"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1663,7 +1717,7 @@
       <c r="E10" s="13">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1672,13 +1726,15 @@
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="35">
-        <v>0.40379999999999999</v>
-      </c>
-      <c r="J10" s="13"/>
+      <c r="I10" s="49">
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0.27839999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1747,7 @@
       <c r="E11" s="13">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1762,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1719,59 +1775,63 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="6">
+        <v>0.45989999999999998</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.60560000000000003</v>
+      </c>
       <c r="J12" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="39" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="42" t="s">
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1781,8 +1841,8 @@
       <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1794,7 +1854,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1809,7 +1869,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1822,7 +1882,7 @@
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1835,7 +1895,7 @@
       <c r="E17" s="13">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="45"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1846,7 +1906,7 @@
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1859,7 +1919,7 @@
       <c r="E18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="47"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1871,18 +1931,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1895,6 +1943,18 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Scripts to display mAP charts for multi-target training
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B19A734-44B5-4255-8A42-2517EB9D94C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54CEA4-8D8C-4D21-826C-8FDA15E7A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="45">
   <si>
     <t>DA Models</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Multi target - TensorFlow 2</t>
   </si>
   <si>
-    <t>DANN + CVA - Evaluation on Source:</t>
-  </si>
-  <si>
     <t>RO:</t>
   </si>
   <si>
@@ -166,6 +163,15 @@
   </si>
   <si>
     <t>results_tr_Amazon_PA_classification_Amazon_PA</t>
+  </si>
+  <si>
+    <t>PA 69.5% / RO 72.4%</t>
+  </si>
+  <si>
+    <t>RO 87.9% MA 88.7%</t>
+  </si>
+  <si>
+    <t>RO 86.1% PA 81.3%</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,12 +231,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -248,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -422,51 +422,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -506,82 +467,47 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -864,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J5" activeCellId="1" sqref="J11 J5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -879,54 +805,54 @@
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -936,8 +862,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -973,7 +899,7 @@
       <c r="H4" s="11">
         <v>0.71599999999999997</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="3">
         <v>0.35</v>
       </c>
       <c r="J4" s="10">
@@ -998,13 +924,13 @@
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="3">
         <v>0.35499999999999998</v>
       </c>
       <c r="I5" s="11">
         <v>0.89300000000000002</v>
       </c>
-      <c r="J5" s="48">
+      <c r="J5" s="10">
         <v>0.76100000000000001</v>
       </c>
     </row>
@@ -1029,7 +955,7 @@
       <c r="H6" s="3">
         <v>0.51300000000000001</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="3">
         <v>0.81299999999999994</v>
       </c>
       <c r="J6" s="11">
@@ -1038,7 +964,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1053,7 +979,7 @@
         <v>0.73499999999999999</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -1147,13 +1073,13 @@
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="47">
-        <v>0.433</v>
-      </c>
-      <c r="J10" s="10">
-        <v>0.59799999999999998</v>
+        <v>42</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1174,14 +1100,14 @@
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="47">
-        <v>0.24199999999999999</v>
+      <c r="H11" s="24">
+        <v>0.30199999999999999</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="48">
-        <v>0.74299999999999999</v>
+        <v>43</v>
+      </c>
+      <c r="J11" s="25">
+        <v>0.25600000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1202,59 +1128,59 @@
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="3">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="I12" s="47">
-        <v>0.81100000000000005</v>
+      <c r="H12" s="21">
+        <v>0.52</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.79300000000000004</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="38" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="41" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1264,8 +1190,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1298,11 +1224,15 @@
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="13"/>
+      <c r="H16" s="4">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0.623</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="35"/>
@@ -1352,90 +1282,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="23"/>
-    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="24">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F10:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1447,7 +1319,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:J14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1462,48 +1334,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1513,8 +1385,8 @@
       <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1487,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1630,7 +1502,7 @@
         <v>0.60189999999999999</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -1726,11 +1598,11 @@
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="49">
-        <v>0.20830000000000001</v>
+      <c r="I10" s="6">
+        <v>0.36380000000000001</v>
       </c>
       <c r="J10" s="13">
-        <v>0.27839999999999998</v>
+        <v>0.32269999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1752,13 +1624,13 @@
         <v>4</v>
       </c>
       <c r="H11" s="6">
-        <v>0.24479999999999999</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="13">
-        <v>0.33129999999999998</v>
+        <v>0.24210000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1779,59 +1651,59 @@
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="6">
-        <v>0.45989999999999998</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.60560000000000003</v>
+      <c r="H12" s="22">
+        <v>0.45750000000000002</v>
+      </c>
+      <c r="I12" s="22">
+        <v>0.66339999999999999</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="38" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="41" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1841,8 +1713,8 @@
       <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +1778,7 @@
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1791,7 @@
       <c r="E18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1931,6 +1803,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1943,18 +1827,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1982,106 +1854,106 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balanced datasets training experiments
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54CEA4-8D8C-4D21-826C-8FDA15E7A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBB8FB0-CF53-4B5D-BA06-0BCEBAE0B5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
     <sheet name="F1-Score" sheetId="1" r:id="rId2"/>
-    <sheet name="Files and experiments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="25">
   <si>
     <t>DA Models</t>
   </si>
@@ -90,95 +89,35 @@
     <t>Multi target - TensorFlow 2</t>
   </si>
   <si>
-    <t>RO:</t>
-  </si>
-  <si>
-    <t>1-Tr: RO, Ts: RO (baseline)</t>
-  </si>
-  <si>
-    <t>2-Tr: RO-&gt;PA,MA, Ts: PA (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>3-Tr: RO-&gt;PA,MA, Ts: MA (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>4-Tr: RO-&gt;PA,MA, Ts: RO (domain adaptation multi-target validating on source)</t>
-  </si>
-  <si>
-    <t>MA:</t>
-  </si>
-  <si>
-    <t>1-Tr: MA, Ts: MA (baseline)</t>
-  </si>
-  <si>
-    <t>2-Tr: MA-&gt;RO,PA, Ts: RO (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>3-Tr: MA-&gt;RO,PA, Ts: PA (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>4-Tr: MA-&gt;RO,PA, Ts: MA (domain adaptation multi-target validating on source)</t>
-  </si>
-  <si>
-    <t>PA:</t>
-  </si>
-  <si>
-    <t>1-Tr: PA, Ts: PA (baseline)</t>
-  </si>
-  <si>
-    <t>2-Tr: PA-&gt;RO,MA, Ts: RO (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>3-Tr: PA-&gt;RO,MA, Ts: MA (domain adaptation multi-target)</t>
-  </si>
-  <si>
-    <t>4-Tr: PA-&gt;RO,MA, Ts: PA (domain adaptation multi-target validating on source)</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Checkpoints</t>
-  </si>
-  <si>
     <t>DANN (Unbalanced)</t>
   </si>
   <si>
-    <t>checkpoint_tr_Cerrado_MA_classification_Cerrado_MA</t>
-  </si>
-  <si>
-    <t>results_tr_Cerrado_MA_classification_Cerrado_MA</t>
-  </si>
-  <si>
-    <t>results_tr_Amazon_RO_classification_Amazon_RO</t>
-  </si>
-  <si>
-    <t>checkpoint_tr_Amazon_RO_classification_Amazon_RO</t>
-  </si>
-  <si>
-    <t>checkpoint_tr_Amazon_PA_classification_Amazon_PA</t>
-  </si>
-  <si>
-    <t>results_tr_Amazon_PA_classification_Amazon_PA</t>
-  </si>
-  <si>
-    <t>PA 69.5% / RO 72.4%</t>
-  </si>
-  <si>
     <t>RO 87.9% MA 88.7%</t>
   </si>
   <si>
     <t>RO 86.1% PA 81.3%</t>
+  </si>
+  <si>
+    <t>X = PA, Y = RO, MA</t>
+  </si>
+  <si>
+    <t>F1 score: avg of 5 runs*</t>
+  </si>
+  <si>
+    <t>PA 69.5% / MA 72.4%</t>
+  </si>
+  <si>
+    <t>Multi target - TensorFlow 2 - Balanced datasets (Source size = Target 1 size = Target 2 size)</t>
+  </si>
+  <si>
+    <t>Multi target - TensorFlow 2 - Unbalanced datasets (Source size = Target 1 size + Target 2 size)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -197,8 +136,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,18 +177,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -427,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -467,23 +401,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -503,11 +422,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -790,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -803,8 +752,8 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -827,32 +776,32 @@
       <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="34"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -862,8 +811,8 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -875,7 +824,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -890,7 +839,7 @@
       <c r="E4" s="10">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -907,7 +856,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -920,7 +869,7 @@
       <c r="E5" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -935,7 +884,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,7 +897,7 @@
       <c r="E6" s="11">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -963,8 +912,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
-        <v>35</v>
+      <c r="A7" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -978,8 +927,8 @@
       <c r="E7" s="10">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>35</v>
+      <c r="F7" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -995,7 +944,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +957,7 @@
       <c r="E8" s="10">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1023,7 +972,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +985,7 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1051,7 +1000,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1066,24 +1015,24 @@
       <c r="E10" s="10">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="21">
+        <v>22</v>
+      </c>
+      <c r="I10" s="32">
         <v>0.57599999999999996</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="34">
         <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1096,22 +1045,22 @@
       <c r="E11" s="10">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="24">
-        <v>0.30199999999999999</v>
+      <c r="H11" s="32">
+        <v>0.254</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="25">
-        <v>0.25600000000000001</v>
+        <v>18</v>
+      </c>
+      <c r="J11" s="34">
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,63 +1073,63 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="35"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="32">
         <v>0.52</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="32">
         <v>0.79300000000000004</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1190,8 +1139,8 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1203,7 +1152,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1218,7 +1167,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1227,7 +1176,7 @@
       <c r="H16" s="4">
         <v>0.72599999999999998</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="31">
         <v>0.37</v>
       </c>
       <c r="J16" s="13">
@@ -1235,7 +1184,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1248,18 +1197,22 @@
       <c r="E17" s="10">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0.64300000000000002</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1272,18 +1225,120 @@
       <c r="E18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="12" t="s">
-        <v>7</v>
+      <c r="H18" s="6">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0.876</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F22" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F23" s="19"/>
+      <c r="G23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0.879</v>
+      </c>
+      <c r="J23" s="39">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F24" s="19"/>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="30">
+        <v>0.432</v>
+      </c>
+      <c r="I24" s="38">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="J24" s="39">
+        <v>0.84299999999999997</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="29">
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F13:J13"/>
@@ -1291,23 +1346,6 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1316,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1331,9 +1369,13 @@
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -1349,33 +1391,33 @@
       <c r="I1" s="27"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="34"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1385,8 +1427,8 @@
       <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1397,8 +1439,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1413,7 +1455,7 @@
       <c r="E4" s="13">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1429,8 +1471,8 @@
         <v>0.4995</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1443,7 +1485,7 @@
       <c r="E5" s="13">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1457,8 +1499,8 @@
         <v>0.44090000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1513,7 @@
       <c r="E6" s="17">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1485,9 +1527,9 @@
         <v>0.6976</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
-        <v>35</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1501,8 +1543,8 @@
       <c r="E7" s="13">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>35</v>
+      <c r="F7" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
@@ -1517,8 +1559,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1531,7 +1573,7 @@
       <c r="E8" s="13">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1545,8 +1587,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1559,7 +1601,7 @@
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1573,8 +1615,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1589,7 +1631,7 @@
       <c r="E10" s="13">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1605,8 +1647,8 @@
         <v>0.32269999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1619,12 +1661,12 @@
       <c r="E11" s="13">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="6">
-        <v>0.27229999999999999</v>
+        <v>0.27110000000000001</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>7</v>
@@ -1633,8 +1675,8 @@
         <v>0.24210000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1647,63 +1689,66 @@
       <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="35"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="31">
         <v>0.45750000000000002</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="31">
         <v>0.66339999999999999</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="29" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1713,8 +1758,8 @@
       <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1725,8 +1770,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1741,20 +1786,24 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
+      <c r="H16" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.1515</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1767,18 +1816,22 @@
       <c r="E17" s="13">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+        <v>20</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.63039999999999996</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0.29349999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
       <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1791,30 +1844,104 @@
       <c r="E18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="15" t="s">
-        <v>7</v>
+      <c r="H18" s="18">
+        <v>0.25519999999999998</v>
+      </c>
+      <c r="I18" s="18">
+        <v>0.47860000000000003</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0.52459999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="33"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F22" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F23" s="19"/>
+      <c r="G23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="38">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="I23" s="38">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="J23" s="39">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="29"/>
+      <c r="G24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="35">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="I24" s="36">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="J24" s="37">
+        <v>0.43099999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
+  <mergeCells count="29">
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="F22:F24"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -1827,6 +1954,18 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1835,129 +1974,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46470600-F60B-4355-835B-9BD29A947D16}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
New experiments and results
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D9424B-7269-4FBC-9FBC-19F8AB4F4DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3AF8D5-3D31-4DD6-A052-29BEC2208178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mAP" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="27">
   <si>
     <t>DA Models</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Multi target - TensorFlow 2 - Balanced datasets - Train on Target (Upper bound DA)</t>
+  </si>
+  <si>
+    <t>Multi target - TensorFlow 2 - Balanced datasets - 2 neuron discriminator</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -355,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -390,9 +399,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -411,11 +417,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,9 +438,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,6 +449,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -731,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -752,48 +770,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -803,8 +821,8 @@
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -816,7 +834,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -831,24 +849,24 @@
       <c r="E4" s="9">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="18">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="J4" s="12">
-        <v>0.67400000000000004</v>
+      <c r="H4" s="35">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0.68600000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -861,22 +879,22 @@
       <c r="E5" s="9">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="18">
         <v>0.35899999999999999</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="35">
         <v>0.86499999999999999</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="19">
         <v>0.77200000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -889,22 +907,22 @@
       <c r="E6" s="10">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="6">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="J6" s="18">
-        <v>0.88400000000000001</v>
+      <c r="H6" s="18">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="J6" s="35">
+        <v>0.88</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -919,7 +937,7 @@
       <c r="E7" s="9">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -936,7 +954,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -949,7 +967,7 @@
       <c r="E8" s="9">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -964,7 +982,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -977,7 +995,7 @@
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -992,7 +1010,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1007,24 +1025,24 @@
       <c r="E10" s="9">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="18">
         <v>0.57599999999999996</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="19">
         <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1037,22 +1055,22 @@
       <c r="E11" s="9">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="6">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="I11" s="25" t="s">
+      <c r="H11" s="18">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="I11" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="19">
         <v>0.51600000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1065,63 +1083,63 @@
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="18">
         <v>0.52</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="18">
         <v>0.79300000000000004</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1131,8 +1149,8 @@
       <c r="E15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1162,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1159,24 +1177,24 @@
       <c r="E16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="38">
         <v>0.72599999999999998</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="39">
         <v>0.37</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="35">
         <v>0.623</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1189,22 +1207,22 @@
       <c r="E17" s="9">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="6">
-        <v>0.254</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="39">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I17" s="39">
         <v>0.86399999999999999</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="35">
         <v>0.64300000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1217,45 +1235,45 @@
       <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="39">
         <v>0.48499999999999999</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="39">
         <v>0.75900000000000001</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="35">
         <v>0.876</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1267,77 +1285,77 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="39">
         <v>0.71899999999999997</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="38">
         <v>0.54900000000000004</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="40">
         <v>0.42199999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="39">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="38">
         <v>0.879</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="40">
         <v>0.60599999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F24" s="33"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="39">
         <v>0.432</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="38">
         <v>0.82099999999999995</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="40">
         <v>0.84299999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F25" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
+      <c r="F25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="32"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="2" t="s">
         <v>3</v>
       </c>
@@ -1349,59 +1367,158 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="6">
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="J28" s="12">
-        <v>0.83199999999999996</v>
+      <c r="H28" s="39">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="I28" s="39">
+        <v>0.32</v>
+      </c>
+      <c r="J28" s="39">
+        <v>0.36799999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="6">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="12">
-        <v>0.85499999999999998</v>
+      <c r="H29" s="39">
+        <v>0.251</v>
+      </c>
+      <c r="I29" s="38">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="J29" s="40">
+        <v>0.55600000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F30" s="33"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="38">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="I30" s="39">
+        <v>0.76</v>
+      </c>
+      <c r="J30" s="35">
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F31" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F32" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F34" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="18">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J34" s="19">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F35" s="24"/>
+      <c r="G35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="18">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="19">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F36" s="24"/>
+      <c r="G36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="18">
         <v>0.70399999999999996</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I36" s="18">
         <v>0.86799999999999999</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J36" s="19" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:J20"/>
+  <mergeCells count="39">
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A13:E13"/>
@@ -1414,23 +1531,11 @@
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1441,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1461,48 +1566,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1512,8 +1617,8 @@
       <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1525,7 +1630,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1540,24 +1645,24 @@
       <c r="E4" s="12">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>0.67200000000000004</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>0.29549999999999998</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="19">
         <v>0.4995</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1570,22 +1675,22 @@
       <c r="E5" s="12">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>0.36799999999999999</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>0.75800000000000001</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="19">
         <v>0.48699999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1598,22 +1703,22 @@
       <c r="E6" s="12">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>0.47660000000000002</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="18">
         <v>0.70720000000000005</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="19">
         <v>0.6976</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1628,24 +1733,24 @@
       <c r="E7" s="12">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="21" t="s">
+      <c r="H7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1658,22 +1763,22 @@
       <c r="E8" s="12">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="21" t="s">
+      <c r="H8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1686,22 +1791,22 @@
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="22" t="s">
+      <c r="H9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1716,24 +1821,24 @@
       <c r="E10" s="12">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="19">
+      <c r="H10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="18">
         <v>0.36380000000000001</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>0.32269999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1746,22 +1851,22 @@
       <c r="E11" s="12">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>0.34899999999999998</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="20">
+      <c r="I11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="19">
         <v>0.20100000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1774,66 +1879,66 @@
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>0.45750000000000002</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="18">
         <v>0.66339999999999999</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
@@ -1843,8 +1948,8 @@
       <c r="E15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
@@ -1856,7 +1961,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1871,24 +1976,24 @@
       <c r="E16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>0.54500000000000004</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="18">
         <v>0.47899999999999998</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="19">
         <v>0.2727</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1901,22 +2006,22 @@
       <c r="E17" s="12">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>0.21560000000000001</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>0.63039999999999996</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="19">
         <v>0.29349999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="13" t="s">
         <v>10</v>
       </c>
@@ -1929,46 +2034,46 @@
       <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="22">
         <v>0.25519999999999998</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="22">
         <v>0.47860000000000003</v>
       </c>
-      <c r="J18" s="24">
+      <c r="J18" s="23">
         <v>0.52459999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="7" t="s">
         <v>3</v>
       </c>
@@ -1980,77 +2085,77 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>0.5</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="18">
         <v>0.14499999999999999</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="19">
         <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>0.22800000000000001</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="18">
         <v>0.70299999999999996</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="19">
         <v>0.255</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="37"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="22">
         <v>0.40899999999999997</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I24" s="22">
         <v>0.41099999999999998</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="23">
         <v>0.43099999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="32"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="2" t="s">
         <v>3</v>
       </c>
@@ -2062,7 +2167,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2079,7 +2184,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2094,7 +2199,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="33"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="1" t="s">
         <v>10</v>
       </c>
@@ -2110,11 +2215,23 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -2127,23 +2244,11 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="F22:F24"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
New experiments and refactor on charts creation
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7490E61-23E6-4F93-90C8-D3F83103C028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E06B5-6DA7-42AC-BD24-B5F296CEAF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="30">
   <si>
     <t>DA Models</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Multi target - TensorFlow 2 - Balanced datasets - 2 neuron fc discriminator</t>
+  </si>
+  <si>
+    <t>Multi target - TensorFlow 2 - Balanced datasets - 3 neuron fc discriminator (5 runs warmup)</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,6 +429,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,12 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -746,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J34" activeCellId="1" sqref="J35 J34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -759,7 +759,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="27.140625" customWidth="1"/>
@@ -767,48 +767,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -818,8 +818,8 @@
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
@@ -831,7 +831,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -846,7 +846,7 @@
       <c r="E4" s="9">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -863,7 +863,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="E5" s="9">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,7 +904,7 @@
       <c r="E6" s="10">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -934,7 +934,7 @@
       <c r="E7" s="9">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="34" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -951,7 +951,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="E8" s="9">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -979,7 +979,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1022,7 +1022,7 @@
       <c r="E10" s="9">
         <v>0.57699999999999996</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1039,7 +1039,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="E11" s="9">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1080,7 @@
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1095,48 +1095,48 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1146,8 +1146,8 @@
       <c r="E15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1174,24 +1174,24 @@
       <c r="E16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="18">
         <v>0.72599999999999998</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="18">
         <v>0.37</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="24">
         <v>0.623</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1204,22 +1204,22 @@
       <c r="E17" s="9">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="18">
         <v>0.26800000000000002</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="18">
         <v>0.86399999999999999</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="19">
         <v>0.64300000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1232,45 +1232,45 @@
       <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="18">
         <v>0.48499999999999999</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="18">
         <v>0.75900000000000001</v>
       </c>
-      <c r="J18" s="39">
+      <c r="J18" s="19">
         <v>0.876</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1282,77 +1282,77 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="18">
         <v>0.71899999999999997</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="27">
         <v>0.54900000000000004</v>
       </c>
-      <c r="J22" s="39">
+      <c r="J22" s="19">
         <v>0.42199999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="18">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="18">
         <v>0.879</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="19">
         <v>0.60599999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F24" s="33"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="18">
         <v>0.432</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="27">
         <v>0.82099999999999995</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="19">
         <v>0.84299999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="2" t="s">
         <v>3</v>
       </c>
@@ -1364,77 +1364,77 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="18">
         <v>0.68799999999999994</v>
       </c>
-      <c r="I28" s="38">
+      <c r="I28" s="18">
         <v>0.32</v>
       </c>
-      <c r="J28" s="38">
+      <c r="J28" s="18">
         <v>0.36799999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="18">
         <v>0.251</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="18">
         <v>0.88200000000000001</v>
       </c>
-      <c r="J29" s="39">
+      <c r="J29" s="19">
         <v>0.55600000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="27">
         <v>0.55200000000000005</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="18">
         <v>0.76</v>
       </c>
-      <c r="J30" s="39">
+      <c r="J30" s="19">
         <v>0.88300000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="31"/>
-      <c r="J32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="33"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="32"/>
       <c r="H33" s="2" t="s">
         <v>3</v>
       </c>
@@ -1446,77 +1446,77 @@
       </c>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="18">
         <v>0.70499999999999996</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="18">
         <v>0.39700000000000002</v>
       </c>
-      <c r="J34" s="38">
+      <c r="J34" s="18">
         <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F35" s="33"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="18">
         <v>0.23899999999999999</v>
       </c>
-      <c r="I35" s="38">
+      <c r="I35" s="18">
         <v>0.88400000000000001</v>
       </c>
-      <c r="J35" s="39">
+      <c r="J35" s="24">
         <v>0.72399999999999998</v>
       </c>
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F36" s="33"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="18">
         <v>0.48099999999999998</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="18">
         <v>0.79200000000000004</v>
       </c>
-      <c r="J36" s="39">
+      <c r="J36" s="19">
         <v>0.86899999999999999</v>
       </c>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F37" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="29"/>
+      <c r="F37" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H38" s="31" t="s">
+      <c r="H38" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I38" s="31"/>
-      <c r="J38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F39" s="30"/>
-      <c r="G39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="32"/>
       <c r="H39" s="2" t="s">
         <v>3</v>
       </c>
@@ -1528,54 +1528,136 @@
       </c>
     </row>
     <row r="40" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F40" s="33" t="s">
+      <c r="F40" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="18" t="s">
-        <v>7</v>
+      <c r="H40" s="18">
+        <v>0.75700000000000001</v>
       </c>
       <c r="I40" s="18">
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="J40" s="19">
-        <v>0.83199999999999996</v>
+        <v>0.255</v>
+      </c>
+      <c r="J40" s="18">
+        <v>0.38300000000000001</v>
       </c>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F41" s="33"/>
+      <c r="F41" s="34"/>
       <c r="G41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="18">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>7</v>
+      <c r="H41" s="27">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I41" s="18">
+        <v>0.88100000000000001</v>
       </c>
       <c r="J41" s="19">
-        <v>0.85499999999999998</v>
+        <v>0.53900000000000003</v>
       </c>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="F42" s="33"/>
+      <c r="F42" s="34"/>
       <c r="G42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H42" s="18">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="I42" s="18">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="J42" s="19">
+        <v>0.83799999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F43" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F44" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="32"/>
+      <c r="J44" s="33"/>
+    </row>
+    <row r="45" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F45" s="31"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F46" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="18">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J46" s="19">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F47" s="34"/>
+      <c r="G47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="18">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="19">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F48" s="34"/>
+      <c r="G48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="18">
         <v>0.70399999999999996</v>
       </c>
-      <c r="I42" s="18">
+      <c r="I48" s="18">
         <v>0.86799999999999999</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="J48" s="19" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="49">
     <mergeCell ref="F31:J31"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
@@ -1610,16 +1692,21 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="F28:F30"/>
     <mergeCell ref="F37:J37"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="G38:G39"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="F28:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1650,48 +1737,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1701,8 +1788,8 @@
       <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1801,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1729,7 +1816,7 @@
       <c r="E4" s="12">
         <v>0.57969999999999999</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1746,7 +1833,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1759,7 +1846,7 @@
       <c r="E5" s="12">
         <v>0.53759999999999997</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1774,7 +1861,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1787,7 +1874,7 @@
       <c r="E6" s="12">
         <v>0.73850000000000005</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1802,7 +1889,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1817,7 +1904,7 @@
       <c r="E7" s="12">
         <v>0.60189999999999999</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="34" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1834,7 +1921,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1847,7 +1934,7 @@
       <c r="E8" s="12">
         <v>0.52090000000000003</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1862,7 +1949,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1875,7 +1962,7 @@
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1977,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1905,7 +1992,7 @@
       <c r="E10" s="12">
         <v>0.45429999999999998</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1922,7 +2009,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1935,7 +2022,7 @@
       <c r="E11" s="12">
         <v>0.55669999999999997</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +2037,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1963,7 +2050,7 @@
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1978,51 +2065,51 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
@@ -2032,8 +2119,8 @@
       <c r="E15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
@@ -2045,7 +2132,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2060,7 +2147,7 @@
       <c r="E16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -2077,7 +2164,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +2177,7 @@
       <c r="E17" s="12">
         <v>0.59819999999999995</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2105,7 +2192,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="13" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2205,7 @@
       <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="13" t="s">
         <v>10</v>
       </c>
@@ -2133,31 +2220,31 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="7" t="s">
         <v>3</v>
       </c>
@@ -2169,7 +2256,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2186,7 +2273,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
@@ -2201,7 +2288,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="37"/>
+      <c r="F24" s="38"/>
       <c r="G24" s="13" t="s">
         <v>10</v>
       </c>
@@ -2216,30 +2303,30 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="2" t="s">
         <v>3</v>
       </c>
@@ -2251,7 +2338,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2268,7 +2355,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2283,7 +2370,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Adding Batch normalization to discriminator
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizm\Documents\workspace\projects\FC-DANN_DA_For_CD_MultiTarget_TF2\FC-DANN_DA_For_CD_MultiTarget_TF2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E06B5-6DA7-42AC-BD24-B5F296CEAF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9D58F-5806-4290-B2AD-25D3EE9BD9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="31">
   <si>
     <t>DA Models</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Multi target - TensorFlow 2 - Balanced datasets - 3 neuron fc discriminator (5 runs warmup)</t>
+  </si>
+  <si>
+    <t>Multi target - TensorFlow 2 - Balanced datasets - 3 neuron fc discriminator (1 run warmup)</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -464,6 +467,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -746,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34785D2B-B6A3-4212-8E7C-08AD6B2EDF48}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F6"/>
+    <sheetView tabSelected="1" topLeftCell="B32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -853,13 +859,13 @@
         <v>3</v>
       </c>
       <c r="H4" s="24">
-        <v>0.72799999999999998</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="I4" s="18">
-        <v>0.39600000000000002</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J4" s="19">
-        <v>0.68600000000000005</v>
+        <v>0.71799999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -881,13 +887,13 @@
         <v>4</v>
       </c>
       <c r="H5" s="18">
-        <v>0.35899999999999999</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="I5" s="24">
-        <v>0.86499999999999999</v>
+        <v>0.876</v>
       </c>
       <c r="J5" s="19">
-        <v>0.77200000000000002</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -909,13 +915,13 @@
         <v>5</v>
       </c>
       <c r="H6" s="18">
-        <v>0.50600000000000001</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="I6" s="18">
-        <v>0.74099999999999999</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="J6" s="24">
-        <v>0.88</v>
+        <v>0.86499999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1576,7 +1582,7 @@
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F43" s="28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G43" s="29"/>
       <c r="H43" s="29"/>
@@ -1616,14 +1622,12 @@
       <c r="G46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>7</v>
-      </c>
+      <c r="H46" s="18"/>
       <c r="I46" s="18">
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="J46" s="19">
-        <v>0.83199999999999996</v>
+        <v>0.438</v>
+      </c>
+      <c r="J46" s="18">
+        <v>0.61899999999999999</v>
       </c>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.2">
@@ -1631,14 +1635,12 @@
       <c r="G47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H47" s="18">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="I47" s="18" t="s">
-        <v>7</v>
-      </c>
+      <c r="H47" s="39">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="I47" s="18"/>
       <c r="J47" s="19">
-        <v>0.85499999999999998</v>
+        <v>0.51200000000000001</v>
       </c>
     </row>
     <row r="48" spans="6:10" x14ac:dyDescent="0.2">
@@ -1647,17 +1649,102 @@
         <v>10</v>
       </c>
       <c r="H48" s="18">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="I48" s="18">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F49" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="30"/>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F50" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="32"/>
+      <c r="J50" s="33"/>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F51" s="31"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F52" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="18">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J52" s="19">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F53" s="34"/>
+      <c r="G53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="18">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I53" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="19">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F54" s="34"/>
+      <c r="G54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="18">
         <v>0.70399999999999996</v>
       </c>
-      <c r="I48" s="18">
+      <c r="I54" s="18">
         <v>0.86799999999999999</v>
       </c>
-      <c r="J48" s="19" t="s">
+      <c r="J54" s="19" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="54">
+    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="F46:F48"/>
     <mergeCell ref="F31:J31"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
@@ -1692,11 +1779,11 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F43:J43"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F49:J49"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="F52:F54"/>
     <mergeCell ref="F25:J25"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="G26:G27"/>

</xml_diff>